<commit_message>
lots of work on historical estimates
</commit_message>
<xml_diff>
--- a/data/historical_estimates/raw/Barlow_etal_1994_Table3.xlsx
+++ b/data/historical_estimates/raw/Barlow_etal_1994_Table3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/ca_set_gillnet_bycatch/data/historical_estimates/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A31A9F2-B48F-6E45-AA23-750BF17B88B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5221C61C-4D8C-C84D-A49A-CE32DF19FB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="25260" windowHeight="23700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="25260" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
   <si>
     <t>Effort</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>Barlow et al. 1994</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>table</t>
   </si>
 </sst>
 </file>
@@ -145,9 +157,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,9 +197,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -220,26 +232,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,26 +267,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,508 +443,612 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1">
+      <c r="E1" s="1">
         <v>1983</v>
       </c>
-      <c r="D1" s="1">
+      <c r="F1" s="1">
         <v>1984</v>
       </c>
-      <c r="E1" s="1">
+      <c r="G1" s="1">
         <v>1985</v>
       </c>
-      <c r="F1" s="1">
+      <c r="H1" s="1">
         <v>1986</v>
       </c>
-      <c r="G1" s="1">
+      <c r="I1" s="1">
         <v>1987</v>
       </c>
-      <c r="H1" s="1">
+      <c r="J1" s="1">
         <v>1990</v>
       </c>
-      <c r="I1" s="1">
+      <c r="K1" s="1">
         <v>1991</v>
       </c>
-      <c r="J1" s="1">
+      <c r="L1" s="1">
         <v>1992</v>
       </c>
-      <c r="K1" s="1">
+      <c r="M1" s="1">
         <v>1993</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>26210</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>37155</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>39104</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>39497</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>29623</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>8070</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>22300</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>16900</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>16300</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>3041</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>7089</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>5468</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>5380</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>962</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>1723</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>1499</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>2107</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>978</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>406</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>2231</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>2155</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>2641</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>0.05</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>0.1</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>0.128</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>0.16200000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>14</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>19</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>33</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>16</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>13</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>5</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>6</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
       <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>2</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>76</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>69</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>84</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>90</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>174</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>67</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>149</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>340</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>31</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>66</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>148</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>103</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>156</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>30</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>43</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>93</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>13</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>3</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>7</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>3</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>303</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>226</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>227</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>197</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>34</v>
-      </c>
-      <c r="H12">
-        <v>44</v>
-      </c>
-      <c r="I12">
-        <v>38</v>
       </c>
       <c r="J12">
         <v>44</v>
       </c>
       <c r="K12">
+        <v>38</v>
+      </c>
+      <c r="L12">
+        <v>44</v>
+      </c>
+      <c r="M12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
       <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>17</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>3427</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>2244</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>2207</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>4288</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>2722</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>847</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>1858</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>3255</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>1984</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>834</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>1138</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>1886</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>2028</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>903</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>392</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>559</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>1136</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>480</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>17</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>144</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>26</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>51</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>33</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
       <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added effort estimates to historical work
</commit_message>
<xml_diff>
--- a/data/historical_estimates/raw/Barlow_etal_1994_Table3.xlsx
+++ b/data/historical_estimates/raw/Barlow_etal_1994_Table3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/ca_set_gillnet_bycatch/data/historical_estimates/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5221C61C-4D8C-C84D-A49A-CE32DF19FB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65671F37-0B28-8B43-A79D-1371C7D96F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="25260" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>